<commit_message>
Initial upload of models
</commit_message>
<xml_diff>
--- a/MSFT Model.xlsx
+++ b/MSFT Model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kerem\OneDrive\Masaüstü\Models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6000B74-C686-40EB-B60B-6CAF7E7C41F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{367D8EC9-2351-4397-9460-3DB871C117B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25848" yWindow="624" windowWidth="32016" windowHeight="15924" xr2:uid="{64BEE0EA-45A1-4490-9445-11F5F6D37C44}"/>
+    <workbookView xWindow="11388" yWindow="1200" windowWidth="46080" windowHeight="15048" xr2:uid="{64BEE0EA-45A1-4490-9445-11F5F6D37C44}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -1210,7 +1210,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1293,7 +1293,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3333,6 +3332,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="1162294175"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -6356,7 +6356,7 @@
   <dimension ref="B2:X96"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Y24" sqref="Y24"/>
+      <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -7184,24 +7184,24 @@
         <v>16</v>
       </c>
       <c r="E31" s="11">
-        <f>F30/E27</f>
-        <v>0.37272143163105043</v>
+        <f>E30/E27</f>
+        <v>0.31074199228975297</v>
       </c>
       <c r="F31" s="11">
-        <f>G30/F27</f>
-        <v>0.3321884299187976</v>
+        <f t="shared" ref="F31:I31" si="4">F30/F27</f>
+        <v>0.31598325515710901</v>
       </c>
       <c r="G31" s="11">
-        <f>H30/G27</f>
-        <v>0.34973456338626335</v>
+        <f t="shared" si="4"/>
+        <v>0.31079914116508978</v>
       </c>
       <c r="H31" s="11">
-        <f>I30/H27</f>
-        <v>0.35831545108150226</v>
+        <f t="shared" si="4"/>
+        <v>0.30235556172028621</v>
       </c>
       <c r="I31" s="11">
-        <f>J30/I27</f>
-        <v>0.37068942937058963</v>
+        <f t="shared" si="4"/>
+        <v>0.31176257613834818</v>
       </c>
       <c r="J31" s="11">
         <f>J30/J27</f>
@@ -7216,11 +7216,11 @@
         <v>0.32000000000000006</v>
       </c>
       <c r="M31" s="11">
-        <f t="shared" ref="M31" si="4">M30/M27</f>
+        <f t="shared" ref="M31" si="5">M30/M27</f>
         <v>0.32000000000000006</v>
       </c>
       <c r="N31" s="11">
-        <f t="shared" ref="N31" si="5">N30/N27</f>
+        <f t="shared" ref="N31" si="6">N30/N27</f>
         <v>0.32</v>
       </c>
     </row>
@@ -7229,19 +7229,19 @@
         <v>65</v>
       </c>
       <c r="E33" s="8">
-        <f t="shared" ref="E33:H33" si="6">E27-E30</f>
+        <f t="shared" ref="E33:H33" si="7">E27-E30</f>
         <v>115856</v>
       </c>
       <c r="F33" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>135620</v>
       </c>
       <c r="G33" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>146052</v>
       </c>
       <c r="H33" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>171008</v>
       </c>
       <c r="I33" s="8">
@@ -7261,11 +7261,11 @@
         <v>297736.21222505602</v>
       </c>
       <c r="M33" s="8">
-        <f t="shared" ref="M33:N33" si="7">M27-M30</f>
+        <f t="shared" ref="M33:N33" si="8">M27-M30</f>
         <v>343885.32511993963</v>
       </c>
       <c r="N33" s="8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>393748.69726233091</v>
       </c>
     </row>
@@ -7278,39 +7278,39 @@
         <v>0.68925800771024703</v>
       </c>
       <c r="F34" s="11">
-        <f t="shared" ref="F34:N34" si="8">F33/F27</f>
+        <f t="shared" ref="F34:N34" si="9">F33/F27</f>
         <v>0.68401674484289099</v>
       </c>
       <c r="G34" s="11">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.68920085883491022</v>
       </c>
       <c r="H34" s="11">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.69764443827971379</v>
       </c>
       <c r="I34" s="11">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.68823742386165188</v>
       </c>
       <c r="J34" s="11">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.68</v>
       </c>
       <c r="K34" s="11">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.67999999999999994</v>
       </c>
       <c r="L34" s="11">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.68</v>
       </c>
       <c r="M34" s="11">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.67999999999999994</v>
       </c>
       <c r="N34" s="11">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.67999999999999994</v>
       </c>
     </row>
@@ -7363,39 +7363,39 @@
         <v>0.15006425205844556</v>
       </c>
       <c r="F37" s="11">
-        <f t="shared" ref="F37:I37" si="9">F36/F27</f>
+        <f t="shared" ref="F37:I37" si="10">F36/F27</f>
         <v>0.13983456902204064</v>
       </c>
       <c r="G37" s="11">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.14314229761932851</v>
       </c>
       <c r="H37" s="11">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.13081241177862452</v>
       </c>
       <c r="I37" s="11">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.11669932274140649</v>
       </c>
       <c r="J37" s="11">
-        <f t="shared" ref="J37" si="10">J36/J27</f>
+        <f t="shared" ref="J37" si="11">J36/J27</f>
         <v>0.12</v>
       </c>
       <c r="K37" s="11">
-        <f t="shared" ref="K37" si="11">K36/K27</f>
+        <f t="shared" ref="K37" si="12">K36/K27</f>
         <v>0.11000000000000001</v>
       </c>
       <c r="L37" s="11">
-        <f t="shared" ref="L37" si="12">L36/L27</f>
+        <f t="shared" ref="L37" si="13">L36/L27</f>
         <v>0.105</v>
       </c>
       <c r="M37" s="11">
-        <f t="shared" ref="M37" si="13">M36/M27</f>
+        <f t="shared" ref="M37" si="14">M36/M27</f>
         <v>0.105</v>
       </c>
       <c r="N37" s="11">
-        <f t="shared" ref="N37" si="14">N36/N27</f>
+        <f t="shared" ref="N37" si="15">N36/N27</f>
         <v>0.105</v>
       </c>
     </row>
@@ -7431,11 +7431,11 @@
         <v>45536.126575596798</v>
       </c>
       <c r="M39" s="8">
-        <f t="shared" ref="M39:N39" si="15">M27*0.1</f>
+        <f t="shared" ref="M39:N39" si="16">M27*0.1</f>
         <v>50571.3713411676</v>
       </c>
       <c r="N39" s="8">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>57904.220185636907</v>
       </c>
       <c r="P39" s="8"/>
@@ -7449,39 +7449,39 @@
         <v>0.12324496692208843</v>
       </c>
       <c r="F40" s="11">
-        <f t="shared" ref="F40:I40" si="16">F39/F27</f>
+        <f t="shared" ref="F40:I40" si="17">F39/F27</f>
         <v>0.12362939426035205</v>
       </c>
       <c r="G40" s="11">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.12832975485454073</v>
       </c>
       <c r="H40" s="11">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.12038903076835208</v>
       </c>
       <c r="I40" s="11">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.11531853871164686</v>
       </c>
       <c r="J40" s="11">
-        <f t="shared" ref="J40" si="17">J39/J27</f>
+        <f t="shared" ref="J40" si="18">J39/J27</f>
         <v>0.109</v>
       </c>
       <c r="K40" s="11">
-        <f t="shared" ref="K40" si="18">K39/K27</f>
+        <f t="shared" ref="K40" si="19">K39/K27</f>
         <v>0.1055</v>
       </c>
       <c r="L40" s="11">
-        <f t="shared" ref="L40" si="19">L39/L27</f>
+        <f t="shared" ref="L40" si="20">L39/L27</f>
         <v>0.104</v>
       </c>
       <c r="M40" s="11">
-        <f t="shared" ref="M40" si="20">M39/M27</f>
+        <f t="shared" ref="M40" si="21">M39/M27</f>
         <v>0.1</v>
       </c>
       <c r="N40" s="11">
-        <f t="shared" ref="N40" si="21">N39/N27</f>
+        <f t="shared" ref="N40" si="22">N39/N27</f>
         <v>0.1</v>
       </c>
     </row>
@@ -7490,19 +7490,19 @@
         <v>13</v>
       </c>
       <c r="E42" s="8">
-        <f t="shared" ref="E42:H42" si="22">E33-E36-E39</f>
+        <f t="shared" ref="E42:H42" si="23">E33-E36-E39</f>
         <v>69916</v>
       </c>
       <c r="F42" s="8">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>83383</v>
       </c>
       <c r="G42" s="8">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>88523</v>
       </c>
       <c r="H42" s="8">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>109433</v>
       </c>
       <c r="I42" s="8">
@@ -7518,7 +7518,7 @@
         <v>175338.74522739998</v>
       </c>
       <c r="L42" s="8">
-        <f t="shared" ref="L42" si="23">L33-L36-L39</f>
+        <f t="shared" ref="L42" si="24">L33-L36-L39</f>
         <v>206226.11170294322</v>
       </c>
       <c r="M42" s="8">
@@ -7535,43 +7535,43 @@
         <v>16</v>
       </c>
       <c r="E43" s="11">
-        <f t="shared" ref="E43:N43" si="24">E42/E27</f>
+        <f t="shared" ref="E43:N43" si="25">E42/E27</f>
         <v>0.41594878872971303</v>
       </c>
       <c r="F43" s="11">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>0.4205527815604983</v>
       </c>
       <c r="G43" s="11">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>0.41772880636104098</v>
       </c>
       <c r="H43" s="11">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>0.44644299573273716</v>
       </c>
       <c r="I43" s="11">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>0.45621956240859851</v>
       </c>
       <c r="J43" s="11">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>0.45100000000000001</v>
       </c>
       <c r="K43" s="11">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>0.46449999999999991</v>
       </c>
       <c r="L43" s="11">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>0.47100000000000003</v>
       </c>
       <c r="M43" s="11">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>0.47499999999999992</v>
       </c>
       <c r="N43" s="11">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>0.47499999999999998</v>
       </c>
     </row>
@@ -7624,39 +7624,39 @@
         <v>0.14061159105211968</v>
       </c>
       <c r="F46" s="11">
-        <f t="shared" ref="F46:I46" si="25">F45/F42</f>
+        <f t="shared" ref="F46:I46" si="26">F45/F42</f>
         <v>0.13165753211086192</v>
       </c>
       <c r="G46" s="11">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>0.19147566169244151</v>
       </c>
       <c r="H46" s="11">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>0.17957106174554294</v>
       </c>
       <c r="I46" s="11">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>0.16957394497697001</v>
       </c>
       <c r="J46" s="11">
-        <f t="shared" ref="J46" si="26">J45/J42</f>
+        <f t="shared" ref="J46" si="27">J45/J42</f>
         <v>0.185</v>
       </c>
       <c r="K46" s="11">
-        <f t="shared" ref="K46" si="27">K45/K42</f>
+        <f t="shared" ref="K46" si="28">K45/K42</f>
         <v>0.185</v>
       </c>
       <c r="L46" s="11">
-        <f t="shared" ref="L46" si="28">L45/L42</f>
+        <f t="shared" ref="L46" si="29">L45/L42</f>
         <v>0.19</v>
       </c>
       <c r="M46" s="11">
-        <f t="shared" ref="M46" si="29">M45/M42</f>
+        <f t="shared" ref="M46" si="30">M45/M42</f>
         <v>0.2</v>
       </c>
       <c r="N46" s="11">
-        <f t="shared" ref="N46" si="30">N45/N42</f>
+        <f t="shared" ref="N46" si="31">N45/N42</f>
         <v>0.21</v>
       </c>
     </row>
@@ -7763,43 +7763,43 @@
         <v>16</v>
       </c>
       <c r="E51" s="11">
-        <f t="shared" ref="E51:N51" si="31">E50/E27</f>
+        <f t="shared" ref="E51:N51" si="32">E50/E27</f>
         <v>6.9523106943981727E-2</v>
       </c>
       <c r="F51" s="11">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>7.2930851868663937E-2</v>
       </c>
       <c r="G51" s="11">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>6.5408300497841118E-2</v>
       </c>
       <c r="H51" s="11">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>9.0922071458294243E-2</v>
       </c>
       <c r="I51" s="11">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>0.12122857832488534</v>
       </c>
       <c r="J51" s="11">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>0.14492329929853912</v>
       </c>
       <c r="K51" s="11">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>0.14549558092773107</v>
       </c>
       <c r="L51" s="11">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>0.13606391213433588</v>
       </c>
       <c r="M51" s="11">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>0.11427012534225611</v>
       </c>
       <c r="N51" s="11">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>9.7803251384638412E-2</v>
       </c>
     </row>
@@ -7812,39 +7812,39 @@
         <v>0.56667636504703711</v>
       </c>
       <c r="F52" s="11">
-        <f t="shared" ref="F52:I52" si="32">F50/F54</f>
+        <f t="shared" ref="F52:I52" si="33">F50/F54</f>
         <v>0.60537553378548103</v>
       </c>
       <c r="G52" s="11">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>0.49315117230583128</v>
       </c>
       <c r="H52" s="11">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>0.50109045124446339</v>
       </c>
       <c r="I52" s="11">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>0.52908552927142882</v>
       </c>
       <c r="J52" s="11">
-        <f t="shared" ref="J52:N52" si="33">J50/J54</f>
+        <f t="shared" ref="J52:N52" si="34">J50/J54</f>
         <v>0.48099999999999998</v>
       </c>
       <c r="K52" s="11">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>0.47199999999999998</v>
       </c>
       <c r="L52" s="11">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>0.47849999999999998</v>
       </c>
       <c r="M52" s="11">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>0.47849999999999998</v>
       </c>
       <c r="N52" s="11">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>0.47849999999999998</v>
       </c>
     </row>
@@ -7951,43 +7951,43 @@
         <v>16</v>
       </c>
       <c r="E58" s="14">
-        <f t="shared" ref="E58:N58" si="34">E57/E27</f>
+        <f t="shared" ref="E58:N58" si="35">E57/E27</f>
         <v>-5.5923087906334778E-3</v>
       </c>
       <c r="F58" s="14">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>2.2696323195642307E-3</v>
       </c>
       <c r="G58" s="14">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>-1.1278106788099002E-2</v>
       </c>
       <c r="H58" s="14">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>7.4248741443036529E-3</v>
       </c>
       <c r="I58" s="14">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>-1.8990217375871421E-2</v>
       </c>
       <c r="J58" s="14">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>-6.0000000000000001E-3</v>
       </c>
       <c r="K58" s="14">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>-4.0000000000000001E-3</v>
       </c>
       <c r="L58" s="14">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>-2E-3</v>
       </c>
       <c r="M58" s="14">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>-2E-3</v>
       </c>
       <c r="N58" s="14">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>1E-3</v>
       </c>
     </row>
@@ -7996,43 +7996,43 @@
         <v>21</v>
       </c>
       <c r="E59" s="14">
-        <f t="shared" ref="E59:N59" si="35">E57/(E27-D27)</f>
+        <f t="shared" ref="E59:N59" si="36">E57/(E27-D27)</f>
         <v>-5.5923087906334778E-3</v>
       </c>
       <c r="F59" s="14">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>1.4909548737658207E-2</v>
       </c>
       <c r="G59" s="14">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>-0.17515573470135581</v>
       </c>
       <c r="H59" s="14">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>5.4807721263589002E-2</v>
       </c>
       <c r="I59" s="14">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>-0.14616687612698759</v>
       </c>
       <c r="J59" s="14">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>-4.387771975026411E-2</v>
       </c>
       <c r="K59" s="14">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>-2.9531964198207201E-2</v>
       </c>
       <c r="L59" s="14">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>-1.4505723987920396E-2</v>
       </c>
       <c r="M59" s="14">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>-1.4903225806451615E-2</v>
       </c>
       <c r="N59" s="14">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>7.8965517241379301E-3</v>
       </c>
     </row>
@@ -8082,43 +8082,43 @@
         <v>11</v>
       </c>
       <c r="E62" s="8">
-        <f t="shared" ref="E62:N62" si="36">E27</f>
+        <f t="shared" ref="E62:N62" si="37">E27</f>
         <v>168088</v>
       </c>
       <c r="F62" s="8">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>198270</v>
       </c>
       <c r="G62" s="8">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>211915</v>
       </c>
       <c r="H62" s="8">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>245122</v>
       </c>
       <c r="I62" s="8">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>281724</v>
       </c>
       <c r="J62" s="8">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>326350.33999999997</v>
       </c>
       <c r="K62" s="8">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>377478.46120000002</v>
       </c>
       <c r="L62" s="8">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>437847.37091920001</v>
       </c>
       <c r="M62" s="8">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>505713.713411676</v>
       </c>
       <c r="N62" s="8">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>579042.20185636904</v>
       </c>
     </row>
@@ -8133,39 +8133,39 @@
         <v>0.175317274411775</v>
       </c>
       <c r="F63" s="11">
-        <f t="shared" ref="F63:N63" si="37">(F62-E62)/E62</f>
+        <f t="shared" ref="F63:N63" si="38">(F62-E62)/E62</f>
         <v>0.17956070629670173</v>
       </c>
       <c r="G63" s="11">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>6.8820295556564284E-2</v>
       </c>
       <c r="H63" s="11">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>0.15669962013071279</v>
       </c>
       <c r="I63" s="11">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>0.14932156232406721</v>
       </c>
       <c r="J63" s="11">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>0.15840446678309256</v>
       </c>
       <c r="K63" s="11">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>0.15666636412880727</v>
       </c>
       <c r="L63" s="11">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>0.15992676648963722</v>
       </c>
       <c r="M63" s="11">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>0.15499999999999997</v>
       </c>
       <c r="N63" s="11">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>0.14500000000000005</v>
       </c>
     </row>
@@ -8186,23 +8186,23 @@
         <v>13</v>
       </c>
       <c r="E65" s="8">
-        <f t="shared" ref="E65:N65" si="38">E42</f>
+        <f t="shared" ref="E65:N65" si="39">E42</f>
         <v>69916</v>
       </c>
       <c r="F65" s="8">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>83383</v>
       </c>
       <c r="G65" s="8">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>88523</v>
       </c>
       <c r="H65" s="8">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>109433</v>
       </c>
       <c r="I65" s="8">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>128528</v>
       </c>
       <c r="J65" s="8">
@@ -8210,19 +8210,19 @@
         <v>147184.00334</v>
       </c>
       <c r="K65" s="8">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>175338.74522739998</v>
       </c>
       <c r="L65" s="8">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>206226.11170294322</v>
       </c>
       <c r="M65" s="8">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>240214.01387054607</v>
       </c>
       <c r="N65" s="8">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>275045.04588177527</v>
       </c>
     </row>
@@ -8233,43 +8233,43 @@
       <c r="C66" s="5"/>
       <c r="D66" s="5"/>
       <c r="E66" s="11">
-        <f t="shared" ref="E66:N66" si="39">E65/E62</f>
+        <f t="shared" ref="E66:N66" si="40">E65/E62</f>
         <v>0.41594878872971303</v>
       </c>
       <c r="F66" s="11">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>0.4205527815604983</v>
       </c>
       <c r="G66" s="11">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>0.41772880636104098</v>
       </c>
       <c r="H66" s="11">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>0.44644299573273716</v>
       </c>
       <c r="I66" s="11">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>0.45621956240859851</v>
       </c>
       <c r="J66" s="11">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>0.45100000000000001</v>
       </c>
       <c r="K66" s="11">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>0.46449999999999991</v>
       </c>
       <c r="L66" s="11">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>0.47100000000000003</v>
       </c>
       <c r="M66" s="11">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>0.47499999999999992</v>
       </c>
       <c r="N66" s="11">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>0.47499999999999998</v>
       </c>
     </row>
@@ -8285,43 +8285,43 @@
         <v>14</v>
       </c>
       <c r="E68" s="8">
-        <f t="shared" ref="E68:N68" si="40">E45</f>
+        <f t="shared" ref="E68:N68" si="41">E45</f>
         <v>9831</v>
       </c>
       <c r="F68" s="8">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>10978</v>
       </c>
       <c r="G68" s="8">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>16950</v>
       </c>
       <c r="H68" s="8">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>19651</v>
       </c>
       <c r="I68" s="8">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>21795</v>
       </c>
       <c r="J68" s="8">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>27229.040617899998</v>
       </c>
       <c r="K68" s="8">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>32437.667867068994</v>
       </c>
       <c r="L68" s="8">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>39182.961223559214</v>
       </c>
       <c r="M68" s="8">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>48042.802774109216</v>
       </c>
       <c r="N68" s="8">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>57759.459635172803</v>
       </c>
     </row>
@@ -8332,43 +8332,43 @@
       <c r="C69" s="5"/>
       <c r="D69" s="5"/>
       <c r="E69" s="11">
-        <f t="shared" ref="E69:N69" si="41">E68/E65</f>
+        <f t="shared" ref="E69:N69" si="42">E68/E65</f>
         <v>0.14061159105211968</v>
       </c>
       <c r="F69" s="11">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>0.13165753211086192</v>
       </c>
       <c r="G69" s="11">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>0.19147566169244151</v>
       </c>
       <c r="H69" s="11">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>0.17957106174554294</v>
       </c>
       <c r="I69" s="11">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>0.16957394497697001</v>
       </c>
       <c r="J69" s="11">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>0.185</v>
       </c>
       <c r="K69" s="11">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>0.185</v>
       </c>
       <c r="L69" s="11">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>0.19</v>
       </c>
       <c r="M69" s="11">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>0.2</v>
       </c>
       <c r="N69" s="11">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>0.21</v>
       </c>
     </row>
@@ -8377,43 +8377,43 @@
         <v>23</v>
       </c>
       <c r="E71" s="8">
-        <f t="shared" ref="E71:N71" si="42">E65-E68</f>
+        <f t="shared" ref="E71:N71" si="43">E65-E68</f>
         <v>60085</v>
       </c>
       <c r="F71" s="8">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>72405</v>
       </c>
       <c r="G71" s="8">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>71573</v>
       </c>
       <c r="H71" s="8">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>89782</v>
       </c>
       <c r="I71" s="8">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>106733</v>
       </c>
       <c r="J71" s="8">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>119954.9627221</v>
       </c>
       <c r="K71" s="8">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>142901.07736033099</v>
       </c>
       <c r="L71" s="8">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>167043.150479384</v>
       </c>
       <c r="M71" s="8">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>192171.21109643686</v>
       </c>
       <c r="N71" s="8">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>217285.58624660247</v>
       </c>
     </row>
@@ -8422,43 +8422,43 @@
         <v>18</v>
       </c>
       <c r="E73" s="8">
-        <f t="shared" ref="E73:N73" si="43">E50</f>
+        <f t="shared" ref="E73:N73" si="44">E50</f>
         <v>11686</v>
       </c>
       <c r="F73" s="8">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>14460</v>
       </c>
       <c r="G73" s="8">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>13861</v>
       </c>
       <c r="H73" s="8">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>22287</v>
       </c>
       <c r="I73" s="8">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>34153</v>
       </c>
       <c r="J73" s="8">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>47295.767999999996</v>
       </c>
       <c r="K73" s="8">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>54921.447999999997</v>
       </c>
       <c r="L73" s="8">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>59575.226204999999</v>
       </c>
       <c r="M73" s="8">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>57787.96941885</v>
       </c>
       <c r="N73" s="8">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>56632.210030472997</v>
       </c>
     </row>
@@ -8469,43 +8469,43 @@
       <c r="C74" s="5"/>
       <c r="D74" s="5"/>
       <c r="E74" s="11">
-        <f t="shared" ref="E74:N74" si="44">E73/E62</f>
+        <f t="shared" ref="E74:N74" si="45">E73/E62</f>
         <v>6.9523106943981727E-2</v>
       </c>
       <c r="F74" s="11">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>7.2930851868663937E-2</v>
       </c>
       <c r="G74" s="11">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>6.5408300497841118E-2</v>
       </c>
       <c r="H74" s="11">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>9.0922071458294243E-2</v>
       </c>
       <c r="I74" s="11">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>0.12122857832488534</v>
       </c>
       <c r="J74" s="11">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>0.14492329929853912</v>
       </c>
       <c r="K74" s="11">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>0.14549558092773107</v>
       </c>
       <c r="L74" s="11">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>0.13606391213433588</v>
       </c>
       <c r="M74" s="11">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>0.11427012534225611</v>
       </c>
       <c r="N74" s="11">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>9.7803251384638412E-2</v>
       </c>
     </row>
@@ -8514,43 +8514,43 @@
         <v>19</v>
       </c>
       <c r="E76" s="8">
-        <f t="shared" ref="E76:N76" si="45">E54</f>
+        <f t="shared" ref="E76:N76" si="46">E54</f>
         <v>20622</v>
       </c>
       <c r="F76" s="8">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v>23886</v>
       </c>
       <c r="G76" s="8">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v>28107</v>
       </c>
       <c r="H76" s="8">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v>44477</v>
       </c>
       <c r="I76" s="8">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v>64551</v>
       </c>
       <c r="J76" s="8">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v>98328</v>
       </c>
       <c r="K76" s="8">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v>116359</v>
       </c>
       <c r="L76" s="8">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v>124504.13</v>
       </c>
       <c r="M76" s="8">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v>120769.0061</v>
       </c>
       <c r="N76" s="8">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v>118353.625978</v>
       </c>
     </row>
@@ -8561,43 +8561,43 @@
       <c r="C77" s="5"/>
       <c r="D77" s="5"/>
       <c r="E77" s="11">
-        <f t="shared" ref="E77:N77" si="46">E76/E62</f>
+        <f t="shared" ref="E77:N77" si="47">E76/E62</f>
         <v>0.12268573604302509</v>
       </c>
       <c r="F77" s="11">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>0.12047208352246935</v>
       </c>
       <c r="G77" s="11">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>0.13263336715192411</v>
       </c>
       <c r="H77" s="11">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>0.18144842160230415</v>
       </c>
       <c r="I77" s="11">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>0.22912850875324786</v>
       </c>
       <c r="J77" s="11">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>0.30129584053750336</v>
       </c>
       <c r="K77" s="11">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>0.30825334942315907</v>
       </c>
       <c r="L77" s="11">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>0.28435509327969882</v>
       </c>
       <c r="M77" s="11">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>0.23880903937775572</v>
       </c>
       <c r="N77" s="11">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>0.2043955096857647</v>
       </c>
     </row>
@@ -8606,43 +8606,43 @@
         <v>20</v>
       </c>
       <c r="E79" s="13">
-        <f t="shared" ref="E79:N79" si="47">E57</f>
+        <f t="shared" ref="E79:N79" si="48">E57</f>
         <v>-940</v>
       </c>
       <c r="F79" s="13">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>450</v>
       </c>
       <c r="G79" s="13">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>-2390</v>
       </c>
       <c r="H79" s="13">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>1820</v>
       </c>
       <c r="I79" s="13">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>-5350</v>
       </c>
       <c r="J79" s="13">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>-1958.1020399999998</v>
       </c>
       <c r="K79" s="13">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>-1509.9138448000001</v>
       </c>
       <c r="L79" s="13">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>-875.69474183840009</v>
       </c>
       <c r="M79" s="13">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>-1011.427426823352</v>
       </c>
       <c r="N79" s="13">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>579.04220185636905</v>
       </c>
     </row>
@@ -8653,43 +8653,43 @@
       <c r="C80" s="5"/>
       <c r="D80" s="5"/>
       <c r="E80" s="11">
-        <f t="shared" ref="E80:N80" si="48">E79/E62</f>
+        <f t="shared" ref="E80:N80" si="49">E79/E62</f>
         <v>-5.5923087906334778E-3</v>
       </c>
       <c r="F80" s="11">
-        <f t="shared" si="48"/>
+        <f t="shared" si="49"/>
         <v>2.2696323195642307E-3</v>
       </c>
       <c r="G80" s="11">
-        <f t="shared" si="48"/>
+        <f t="shared" si="49"/>
         <v>-1.1278106788099002E-2</v>
       </c>
       <c r="H80" s="11">
-        <f t="shared" si="48"/>
+        <f t="shared" si="49"/>
         <v>7.4248741443036529E-3</v>
       </c>
       <c r="I80" s="11">
-        <f t="shared" si="48"/>
+        <f t="shared" si="49"/>
         <v>-1.8990217375871421E-2</v>
       </c>
       <c r="J80" s="11">
-        <f t="shared" si="48"/>
+        <f t="shared" si="49"/>
         <v>-6.0000000000000001E-3</v>
       </c>
       <c r="K80" s="11">
-        <f t="shared" si="48"/>
+        <f t="shared" si="49"/>
         <v>-4.0000000000000001E-3</v>
       </c>
       <c r="L80" s="11">
-        <f t="shared" si="48"/>
+        <f t="shared" si="49"/>
         <v>-2E-3</v>
       </c>
       <c r="M80" s="11">
-        <f t="shared" si="48"/>
+        <f t="shared" si="49"/>
         <v>-2E-3</v>
       </c>
       <c r="N80" s="11">
-        <f t="shared" si="48"/>
+        <f t="shared" si="49"/>
         <v>1E-3</v>
       </c>
     </row>
@@ -8759,39 +8759,39 @@
         <v>3.6397601256484696E-2</v>
       </c>
       <c r="F83" s="11">
-        <f t="shared" ref="F83:I83" si="49">F82/F62</f>
+        <f t="shared" ref="F83:I83" si="50">F82/F62</f>
         <v>3.7837292580824126E-2</v>
       </c>
       <c r="G83" s="11">
-        <f t="shared" si="49"/>
+        <f t="shared" si="50"/>
         <v>4.5353089682183892E-2</v>
       </c>
       <c r="H83" s="11">
-        <f t="shared" si="49"/>
+        <f t="shared" si="50"/>
         <v>4.3790439046678793E-2</v>
       </c>
       <c r="I83" s="11">
-        <f t="shared" si="49"/>
+        <f t="shared" si="50"/>
         <v>4.2502591188539135E-2</v>
       </c>
       <c r="J83" s="11">
-        <f t="shared" ref="J83" si="50">J82/J62</f>
+        <f t="shared" ref="J83" si="51">J82/J62</f>
         <v>3.7999999999999999E-2</v>
       </c>
       <c r="K83" s="11">
-        <f t="shared" ref="K83" si="51">K82/K62</f>
+        <f t="shared" ref="K83" si="52">K82/K62</f>
         <v>3.7999999999999999E-2</v>
       </c>
       <c r="L83" s="11">
-        <f t="shared" ref="L83" si="52">L82/L62</f>
+        <f t="shared" ref="L83" si="53">L82/L62</f>
         <v>3.8000000000000006E-2</v>
       </c>
       <c r="M83" s="11">
-        <f t="shared" ref="M83" si="53">M82/M62</f>
+        <f t="shared" ref="M83" si="54">M82/M62</f>
         <v>3.7999999999999999E-2</v>
       </c>
       <c r="N83" s="11">
-        <f t="shared" ref="N83" si="54">N82/N62</f>
+        <f t="shared" ref="N83" si="55">N82/N62</f>
         <v>3.7999999999999999E-2</v>
       </c>
     </row>
@@ -8819,19 +8819,19 @@
         <v>83282.145682100003</v>
       </c>
       <c r="K85" s="8">
-        <f t="shared" ref="K85:N85" si="55">K71+K73-K76-(K79)+K82</f>
+        <f t="shared" ref="K85:N85" si="56">K71+K73-K76-(K79)+K82</f>
         <v>97317.620730730996</v>
       </c>
       <c r="L85" s="8">
-        <f t="shared" si="55"/>
+        <f t="shared" si="56"/>
         <v>119628.14152115201</v>
       </c>
       <c r="M85" s="8">
-        <f t="shared" si="55"/>
+        <f t="shared" si="56"/>
         <v>149418.72295175391</v>
       </c>
       <c r="N85" s="8">
-        <f t="shared" si="55"/>
+        <f t="shared" si="56"/>
         <v>176988.73176776114</v>
       </c>
     </row>
@@ -8846,39 +8846,39 @@
         <v>0.33387273333016038</v>
       </c>
       <c r="F86" s="11">
-        <f t="shared" ref="F86:N86" si="56">F85/F62</f>
+        <f t="shared" ref="F86:N86" si="57">F85/F62</f>
         <v>0.32859232359913249</v>
       </c>
       <c r="G86" s="11">
-        <f t="shared" si="56"/>
+        <f t="shared" si="57"/>
         <v>0.28067857395653917</v>
       </c>
       <c r="H86" s="11">
-        <f t="shared" si="56"/>
+        <f t="shared" si="57"/>
         <v>0.30217605926844593</v>
       </c>
       <c r="I86" s="11">
-        <f t="shared" si="56"/>
+        <f t="shared" si="57"/>
         <v>0.25418494696937427</v>
       </c>
       <c r="J86" s="11">
-        <f t="shared" si="56"/>
+        <f t="shared" si="57"/>
         <v>0.2551924587610358</v>
       </c>
       <c r="K86" s="11">
-        <f t="shared" si="56"/>
+        <f t="shared" si="57"/>
         <v>0.25780973150457198</v>
       </c>
       <c r="L86" s="11">
-        <f t="shared" si="56"/>
+        <f t="shared" si="57"/>
         <v>0.27321881885463711</v>
       </c>
       <c r="M86" s="11">
-        <f t="shared" si="56"/>
+        <f t="shared" si="57"/>
         <v>0.29546108596450038</v>
       </c>
       <c r="N86" s="11">
-        <f t="shared" si="56"/>
+        <f t="shared" si="57"/>
         <v>0.30565774169887372</v>
       </c>
     </row>
@@ -11359,9 +11359,6 @@
       <c r="T25" s="50"/>
       <c r="U25" s="50"/>
       <c r="V25" s="50"/>
-      <c r="AA25" s="52"/>
-      <c r="AB25" s="52"/>
-      <c r="AC25" s="52"/>
     </row>
     <row r="26" spans="2:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="1" t="s">
@@ -11543,9 +11540,6 @@
       </c>
       <c r="F36" s="50"/>
       <c r="G36" s="50"/>
-      <c r="M36" s="52"/>
-      <c r="N36" s="52"/>
-      <c r="O36" s="52"/>
       <c r="T36" s="50"/>
       <c r="U36" s="50"/>
       <c r="V36" s="50"/>
@@ -12032,49 +12026,41 @@
     <sortCondition descending="1" ref="F72:F80"/>
   </sortState>
   <mergeCells count="90">
-    <mergeCell ref="Z37:AD37"/>
-    <mergeCell ref="AA39:AC39"/>
-    <mergeCell ref="Z24:AD24"/>
-    <mergeCell ref="AA30:AC30"/>
-    <mergeCell ref="AA31:AC31"/>
-    <mergeCell ref="AA33:AC33"/>
-    <mergeCell ref="AA34:AC34"/>
-    <mergeCell ref="AA35:AC35"/>
-    <mergeCell ref="AA27:AC27"/>
-    <mergeCell ref="AA28:AC28"/>
-    <mergeCell ref="AA29:AC29"/>
-    <mergeCell ref="T46:V46"/>
-    <mergeCell ref="T47:V47"/>
-    <mergeCell ref="T48:V48"/>
-    <mergeCell ref="T49:V49"/>
-    <mergeCell ref="T50:V50"/>
-    <mergeCell ref="T39:V39"/>
-    <mergeCell ref="T40:V40"/>
-    <mergeCell ref="T41:V41"/>
-    <mergeCell ref="T42:V42"/>
-    <mergeCell ref="T43:V43"/>
-    <mergeCell ref="T34:V34"/>
-    <mergeCell ref="T35:V35"/>
-    <mergeCell ref="T36:V36"/>
-    <mergeCell ref="T37:V37"/>
-    <mergeCell ref="T38:V38"/>
-    <mergeCell ref="T27:V27"/>
-    <mergeCell ref="T28:V28"/>
-    <mergeCell ref="T29:V29"/>
-    <mergeCell ref="T32:V32"/>
-    <mergeCell ref="T33:V33"/>
-    <mergeCell ref="T24:V24"/>
-    <mergeCell ref="T25:V25"/>
-    <mergeCell ref="T26:V26"/>
-    <mergeCell ref="M30:O30"/>
-    <mergeCell ref="M31:O31"/>
-    <mergeCell ref="M32:O32"/>
-    <mergeCell ref="M33:O33"/>
-    <mergeCell ref="M35:O35"/>
-    <mergeCell ref="M24:O24"/>
-    <mergeCell ref="M27:O27"/>
-    <mergeCell ref="M28:O28"/>
-    <mergeCell ref="M29:O29"/>
+    <mergeCell ref="E69:G69"/>
+    <mergeCell ref="E60:G60"/>
+    <mergeCell ref="E63:G63"/>
+    <mergeCell ref="E65:G65"/>
+    <mergeCell ref="D67:H67"/>
+    <mergeCell ref="E64:G64"/>
+    <mergeCell ref="E61:G61"/>
+    <mergeCell ref="E55:G55"/>
+    <mergeCell ref="E57:G57"/>
+    <mergeCell ref="E58:G58"/>
+    <mergeCell ref="E59:G59"/>
+    <mergeCell ref="E42:G42"/>
+    <mergeCell ref="E43:G43"/>
+    <mergeCell ref="E46:G46"/>
+    <mergeCell ref="E47:G47"/>
+    <mergeCell ref="E48:G48"/>
+    <mergeCell ref="E32:G32"/>
+    <mergeCell ref="E34:G34"/>
+    <mergeCell ref="E24:G24"/>
+    <mergeCell ref="E25:G25"/>
+    <mergeCell ref="E26:G26"/>
+    <mergeCell ref="E27:G27"/>
+    <mergeCell ref="E29:G29"/>
+    <mergeCell ref="E28:G28"/>
+    <mergeCell ref="E36:G36"/>
+    <mergeCell ref="E49:G49"/>
+    <mergeCell ref="E50:G50"/>
+    <mergeCell ref="E53:G53"/>
+    <mergeCell ref="E33:G33"/>
+    <mergeCell ref="E35:G35"/>
+    <mergeCell ref="E37:G37"/>
+    <mergeCell ref="E38:G38"/>
+    <mergeCell ref="E39:G39"/>
+    <mergeCell ref="E40:G40"/>
+    <mergeCell ref="E41:G41"/>
     <mergeCell ref="E8:G8"/>
     <mergeCell ref="E17:G17"/>
     <mergeCell ref="E9:G9"/>
@@ -12087,41 +12073,49 @@
     <mergeCell ref="E14:G14"/>
     <mergeCell ref="E18:G18"/>
     <mergeCell ref="E20:G20"/>
-    <mergeCell ref="E36:G36"/>
-    <mergeCell ref="E49:G49"/>
-    <mergeCell ref="E50:G50"/>
-    <mergeCell ref="E53:G53"/>
-    <mergeCell ref="E33:G33"/>
-    <mergeCell ref="E35:G35"/>
-    <mergeCell ref="E37:G37"/>
-    <mergeCell ref="E38:G38"/>
-    <mergeCell ref="E39:G39"/>
-    <mergeCell ref="E40:G40"/>
-    <mergeCell ref="E41:G41"/>
-    <mergeCell ref="E32:G32"/>
-    <mergeCell ref="E34:G34"/>
-    <mergeCell ref="E24:G24"/>
-    <mergeCell ref="E25:G25"/>
-    <mergeCell ref="E26:G26"/>
-    <mergeCell ref="E27:G27"/>
-    <mergeCell ref="E29:G29"/>
-    <mergeCell ref="E28:G28"/>
-    <mergeCell ref="E55:G55"/>
-    <mergeCell ref="E57:G57"/>
-    <mergeCell ref="E58:G58"/>
-    <mergeCell ref="E59:G59"/>
-    <mergeCell ref="E42:G42"/>
-    <mergeCell ref="E43:G43"/>
-    <mergeCell ref="E46:G46"/>
-    <mergeCell ref="E47:G47"/>
-    <mergeCell ref="E48:G48"/>
-    <mergeCell ref="E69:G69"/>
-    <mergeCell ref="E60:G60"/>
-    <mergeCell ref="E63:G63"/>
-    <mergeCell ref="E65:G65"/>
-    <mergeCell ref="D67:H67"/>
-    <mergeCell ref="E64:G64"/>
-    <mergeCell ref="E61:G61"/>
+    <mergeCell ref="M32:O32"/>
+    <mergeCell ref="M33:O33"/>
+    <mergeCell ref="M35:O35"/>
+    <mergeCell ref="M24:O24"/>
+    <mergeCell ref="M27:O27"/>
+    <mergeCell ref="M28:O28"/>
+    <mergeCell ref="M29:O29"/>
+    <mergeCell ref="T24:V24"/>
+    <mergeCell ref="T25:V25"/>
+    <mergeCell ref="T26:V26"/>
+    <mergeCell ref="M30:O30"/>
+    <mergeCell ref="M31:O31"/>
+    <mergeCell ref="T27:V27"/>
+    <mergeCell ref="T28:V28"/>
+    <mergeCell ref="T29:V29"/>
+    <mergeCell ref="T32:V32"/>
+    <mergeCell ref="T33:V33"/>
+    <mergeCell ref="T34:V34"/>
+    <mergeCell ref="T35:V35"/>
+    <mergeCell ref="T36:V36"/>
+    <mergeCell ref="T37:V37"/>
+    <mergeCell ref="T38:V38"/>
+    <mergeCell ref="T39:V39"/>
+    <mergeCell ref="T40:V40"/>
+    <mergeCell ref="T41:V41"/>
+    <mergeCell ref="T42:V42"/>
+    <mergeCell ref="T43:V43"/>
+    <mergeCell ref="T46:V46"/>
+    <mergeCell ref="T47:V47"/>
+    <mergeCell ref="T48:V48"/>
+    <mergeCell ref="T49:V49"/>
+    <mergeCell ref="T50:V50"/>
+    <mergeCell ref="Z37:AD37"/>
+    <mergeCell ref="AA39:AC39"/>
+    <mergeCell ref="Z24:AD24"/>
+    <mergeCell ref="AA30:AC30"/>
+    <mergeCell ref="AA31:AC31"/>
+    <mergeCell ref="AA33:AC33"/>
+    <mergeCell ref="AA34:AC34"/>
+    <mergeCell ref="AA35:AC35"/>
+    <mergeCell ref="AA27:AC27"/>
+    <mergeCell ref="AA28:AC28"/>
+    <mergeCell ref="AA29:AC29"/>
   </mergeCells>
   <conditionalFormatting sqref="R5:AJ5">
     <cfRule type="colorScale" priority="3">

</xml_diff>